<commit_message>
RaFHY pH9 Calcs Corrected, MasterPlot Separates Fitted isotherms
</commit_message>
<xml_diff>
--- a/Sorption Experiments/RaFHY_pH5/RaFHY_pH5_NoScript.xlsx
+++ b/Sorption Experiments/RaFHY_pH5/RaFHY_pH5_NoScript.xlsx
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="138">
   <si>
     <t>Parameters</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>CPS-&gt;Bq No background</t>
+  </si>
+  <si>
+    <t>TotAct</t>
   </si>
 </sst>
 </file>
@@ -9206,16 +9209,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -9232,19 +9235,22 @@
         <v>128</v>
       </c>
       <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
         <v>129</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>130</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>131</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9264,24 +9270,28 @@
         <f>_xlfn.STDEV.S('Bottle Results'!U2:U4)</f>
         <v>6.8093211868441603</v>
       </c>
-      <c r="F2" t="e">
+      <c r="F2">
+        <f>'Bottle Results'!S3</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="e">
         <f>AVERAGE('Bottle Results'!W2:W4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G2" t="e">
+      <c r="H2" t="e">
         <f>_xlfn.STDEV.S('Bottle Results'!W2:W4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <f>AVERAGE('Bottle Results'!D2:D4)</f>
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>_xlfn.STDEV.S('Bottle Results'!D2:D4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -9302,23 +9312,27 @@
         <v>20.80869466222557</v>
       </c>
       <c r="F3">
+        <f>'Bottle Results'!S6</f>
+        <v>2.7062351729187553</v>
+      </c>
+      <c r="G3">
         <f>AVERAGE('Bottle Results'!W5:W7)</f>
         <v>-0.20166722495183589</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <f>_xlfn.STDEV.S('Bottle Results'!W5:W7)</f>
         <v>0.23067501528090892</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <f>AVERAGE('Bottle Results'!D5:D7)</f>
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>_xlfn.STDEV.S('Bottle Results'!D5:D7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -9339,23 +9353,27 @@
         <v>19.001302140550514</v>
       </c>
       <c r="F4">
+        <f>'Bottle Results'!S9</f>
+        <v>5.3988024914288308</v>
+      </c>
+      <c r="G4">
         <f>AVERAGE('Bottle Results'!W8:W10)</f>
         <v>3.0162710475767435E-2</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f>_xlfn.STDEV.S('Bottle Results'!W8:W10)</f>
         <v>0.10558620455582746</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f>AVERAGE('Bottle Results'!D8:D10)</f>
         <v>5</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>_xlfn.STDEV.S('Bottle Results'!D8:D10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -9376,23 +9394,27 @@
         <v>252.37331757908467</v>
       </c>
       <c r="F5">
+        <f>'Bottle Results'!S12</f>
+        <v>27.028182093165853</v>
+      </c>
+      <c r="G5">
         <f>AVERAGE('Bottle Results'!W11:W13)</f>
         <v>0.25851943601113264</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f>_xlfn.STDEV.S('Bottle Results'!W11:W13)</f>
         <v>0.28012241079606082</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>AVERAGE('Bottle Results'!D11:D13)</f>
         <v>5</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f>_xlfn.STDEV.S('Bottle Results'!D11:D13)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -9413,23 +9435,27 @@
         <v>22.653325833680704</v>
       </c>
       <c r="F6">
+        <f>'Bottle Results'!S15</f>
+        <v>53.988024914288303</v>
+      </c>
+      <c r="G6">
         <f>AVERAGE('Bottle Results'!W14:W16)</f>
         <v>0.10236533765624593</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f>_xlfn.STDEV.S('Bottle Results'!W14:W16)</f>
         <v>1.2587972538157445E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f>AVERAGE('Bottle Results'!D14:D16)</f>
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>_xlfn.STDEV.S('Bottle Results'!D14:D16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>500</v>
       </c>
@@ -9450,18 +9476,22 @@
         <v>413.30751725734325</v>
       </c>
       <c r="F7">
+        <f>'Bottle Results'!S18</f>
+        <v>270.62351729187554</v>
+      </c>
+      <c r="G7">
         <f>AVERAGE('Bottle Results'!W17:W20)</f>
         <v>0.12510746358958363</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f>_xlfn.STDEV.S('Bottle Results'!W17:W20)</f>
         <v>4.5817250628471216E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f>AVERAGE('Bottle Results'!D17:D20)</f>
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>_xlfn.STDEV.S('Bottle Results'!D17:D20)</f>
         <v>0</v>
       </c>

</xml_diff>